<commit_message>
actually add cluster chart
</commit_message>
<xml_diff>
--- a/Resources/images/final_visualization.xlsx
+++ b/Resources/images/final_visualization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arischitelli/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arischitelli/Desktop/uo-data-analytics/Portfolio_Project/Resources/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FE8EBE-51FC-5949-B086-8CED224F73D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8145543-DD06-D743-B903-E52EC2A2DC5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="460" windowWidth="19260" windowHeight="16320" xr2:uid="{4853D9B5-3959-0B45-B58E-946C84E40137}"/>
+    <workbookView xWindow="4960" yWindow="460" windowWidth="22080" windowHeight="16320" xr2:uid="{4853D9B5-3959-0B45-B58E-946C84E40137}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>cluster 1</t>
   </si>
@@ -175,12 +175,18 @@
 Biking (16)
 Swimming (14)</t>
   </si>
+  <si>
+    <t>* Largest cluster</t>
+  </si>
+  <si>
+    <t>*Smallest cluster</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,8 +198,14 @@
       <name val="ProximaNova-Regular"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="ProximaNova-Regular"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +227,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,17 +264,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -266,6 +311,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE2FFBC"/>
+      <color rgb="FF788468"/>
       <color rgb="FFFF8C8F"/>
     </mruColors>
   </colors>
@@ -577,272 +624,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E830EE-1424-624F-B4FA-44FFAF63B620}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:14">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:14">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="13"/>
+      <c r="B6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="I6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="K6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" spans="1:14" ht="18">
+      <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B7" s="7">
+        <v>49</v>
+      </c>
+      <c r="C7" s="7">
+        <v>59</v>
+      </c>
+      <c r="D7" s="7">
+        <v>87</v>
+      </c>
+      <c r="E7" s="7">
+        <v>56</v>
+      </c>
+      <c r="F7" s="7">
+        <v>107</v>
+      </c>
+      <c r="G7" s="7">
+        <v>138</v>
+      </c>
+      <c r="H7" s="7">
         <v>57</v>
       </c>
-      <c r="C4" s="1">
-        <v>87</v>
-      </c>
-      <c r="D4" s="1">
-        <v>138</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="I7" s="6">
+        <v>234</v>
+      </c>
+      <c r="J7" s="6">
         <v>29</v>
       </c>
-      <c r="F4" s="1">
-        <v>107</v>
-      </c>
-      <c r="G4" s="1">
-        <v>59</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="K7" s="6">
         <v>76</v>
       </c>
-      <c r="I4" s="1">
-        <v>234</v>
-      </c>
-      <c r="J4" s="1">
-        <v>56</v>
-      </c>
-      <c r="K4" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:14" ht="54">
+      <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B8" s="7">
+        <v>203</v>
+      </c>
+      <c r="C8" s="7">
+        <v>253</v>
+      </c>
+      <c r="D8" s="7">
+        <v>192</v>
+      </c>
+      <c r="E8" s="7">
+        <v>171.4</v>
+      </c>
+      <c r="F8" s="7">
+        <v>120.4</v>
+      </c>
+      <c r="G8" s="7">
+        <v>100.4</v>
+      </c>
+      <c r="H8" s="7">
         <v>71.5</v>
       </c>
-      <c r="C5" s="1">
-        <v>192</v>
-      </c>
-      <c r="D5" s="1">
-        <v>100.4</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="I8" s="6">
+        <v>63.2</v>
+      </c>
+      <c r="J8" s="6">
         <v>62.8</v>
       </c>
-      <c r="F5" s="1">
-        <v>120.4</v>
-      </c>
-      <c r="G5" s="1">
-        <v>253</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="K8" s="6">
         <v>54.6</v>
       </c>
-      <c r="I5" s="1">
-        <v>63.2</v>
-      </c>
-      <c r="J5" s="1">
-        <v>171.4</v>
-      </c>
-      <c r="K5" s="1">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" spans="1:14" ht="124" customHeight="1">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B9" s="7">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>26</v>
+      </c>
+      <c r="F9" s="7">
+        <v>23</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
         <v>16</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="I9" s="6">
+        <v>20</v>
+      </c>
+      <c r="J9" s="6">
         <v>19</v>
       </c>
-      <c r="F6" s="1">
+      <c r="K9" s="6">
+        <v>26</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="1:14" ht="36">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:14" ht="36">
+      <c r="A11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" ht="126">
+      <c r="A12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1">
-        <v>19</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="K12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1">
-        <v>26</v>
-      </c>
-      <c r="K6" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="124" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="13" spans="1:14" ht="36">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="18">
+      <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="I16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="14" customFormat="1" ht="23" customHeight="1">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:14" ht="23" customHeight="1"/>
+    <row r="20" spans="1:14" ht="30" customHeight="1"/>
+    <row r="23" spans="1:14" ht="107" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding pie charts to cluster table
</commit_message>
<xml_diff>
--- a/Resources/images/final_visualization.xlsx
+++ b/Resources/images/final_visualization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arischitelli/Desktop/uo-data-analytics/Portfolio_Project/Resources/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34267AEB-4024-2B4A-92A9-FABDF4D18126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB45EA25-6442-9D49-B316-E253AC4DFBA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="27500" windowHeight="16320" xr2:uid="{4853D9B5-3959-0B45-B58E-946C84E40137}"/>
   </bookViews>
@@ -391,23 +391,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>495300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>88899</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1792986</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1673304</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7972DC8C-639B-1446-BA0B-7644B1614498}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D442EFD6-386C-124B-A4DF-8E1F90BF6E3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -423,8 +423,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="38100" y="5715000"/>
-          <a:ext cx="990600" cy="1297686"/>
+          <a:off x="3276599" y="5511800"/>
+          <a:ext cx="1244601" cy="1381204"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -438,20 +438,20 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>279400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1229713</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1409700</xdr:rowOff>
+      <xdr:colOff>1268046</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1625600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A8D517-DD87-ED42-A3A8-DF4251B98EBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDDFD1A0-16E6-4E48-8ACC-DFAF6D5C62B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -467,8 +467,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1917700" y="5346700"/>
-          <a:ext cx="1204313" cy="1282700"/>
+          <a:off x="1917700" y="5499100"/>
+          <a:ext cx="1242646" cy="1346200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -479,23 +479,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>194732</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>186265</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>469900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1303865</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1393314</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1184300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1739900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{201F1EDA-569E-4E40-8A24-1B66382DA512}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50042612-B9F6-CB48-8605-922CDB73EF03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -503,15 +503,368 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:srcRect l="1872"/>
-        <a:stretch/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3386665" y="5435598"/>
-          <a:ext cx="1109133" cy="1207049"/>
+          <a:off x="114300" y="5689600"/>
+          <a:ext cx="1070000" cy="1270000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>50799</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438062</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1714500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0735D773-79D6-294C-8821-513BEBF0CE1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4775199" y="5499100"/>
+          <a:ext cx="1387263" cy="1435100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>126999</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1441638</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1752600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84E3156-7853-8F41-A855-CEEEE9FF9D2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6375399" y="5410200"/>
+          <a:ext cx="1314639" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1429190</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1778000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35D30636-94E0-BF42-931A-093609A2E8D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886700" y="5397500"/>
+          <a:ext cx="1378390" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1421208</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1752600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDA3923E-5B29-EF4F-B614-2D9F414516EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9372599" y="5410200"/>
+          <a:ext cx="1383109" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1432168</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1651000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8CBBB3-642C-444E-B7F4-7660B92F50FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10858499" y="5448300"/>
+          <a:ext cx="1406769" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1390864</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1676400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69022F56-BC97-214B-AFB0-DC22D95A5223}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12344400" y="5486400"/>
+          <a:ext cx="1314664" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1410240</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1727200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB721C1-29F7-954E-83EE-F0CD5C827123}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13817600" y="5461000"/>
+          <a:ext cx="1359440" cy="1485900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1400907</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1714500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE06B76-258F-2F47-BD39-5D09CF0A4C04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15252699" y="5511800"/>
+          <a:ext cx="1375508" cy="1422400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -820,10 +1173,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E830EE-1424-624F-B4FA-44FFAF63B620}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A3:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -837,7 +1193,7 @@
     <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14">
@@ -1132,6 +1488,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="52" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>